<commit_message>
Removed previous generated outputs
</commit_message>
<xml_diff>
--- a/Input/excel_input.xlsx
+++ b/Input/excel_input.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaldixi\Desktop\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaldixi\PycharmProjects\Github_Jenkins_project\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC25D0D-E9D4-498F-8639-16A233A77F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B7D239-2C21-4C98-86EA-BB1DDDB7BFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Provisioning_TBT" sheetId="6" r:id="rId1"/>
-    <sheet name="ciq_sheet_1" sheetId="4" r:id="rId2"/>
-    <sheet name="ciq_sheet_2" sheetId="5" r:id="rId3"/>
+    <sheet name="values" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="173">
   <si>
     <t>172.16.128.242</t>
   </si>
@@ -547,22 +546,13 @@
     <t>100m</t>
   </si>
   <si>
-    <t>ciq_sheet_1</t>
-  </si>
-  <si>
-    <t>ciq_sheet_2</t>
-  </si>
-  <si>
     <t>Values_File_Name</t>
   </si>
   <si>
-    <t>values_2</t>
-  </si>
-  <si>
-    <t>NOACTION</t>
-  </si>
-  <si>
-    <t>demo_values</t>
+    <t>values</t>
+  </si>
+  <si>
+    <t>smf01_test</t>
   </si>
 </sst>
 </file>
@@ -704,55 +694,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -1111,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E44871-E4D3-47A4-B4BE-B82B60F5F0B5}">
-  <dimension ref="B3:D5"/>
+  <dimension ref="B3:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1132,66 +1074,39 @@
         <v>167</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>168</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>173</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NOACTION">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="NOACTION">
       <formula>NOT(ISERROR(SEARCH("NOACTION",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="CREATE">
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="CREATE">
       <formula>NOT(ISERROR(SEARCH("CREATE",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C5">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="NOACTION">
+  <conditionalFormatting sqref="C4">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="NOACTION">
       <formula>NOT(ISERROR(SEARCH("NOACTION",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="CREATE">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="CREATE">
       <formula>NOT(ISERROR(SEARCH("CREATE",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NOACTION">
-      <formula>NOT(ISERROR(SEARCH("NOACTION",C5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="CREATE">
-      <formula>NOT(ISERROR(SEARCH("CREATE",C5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NOACTION">
-      <formula>NOT(ISERROR(SEARCH("NOACTION",C5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="CREATE">
-      <formula>NOT(ISERROR(SEARCH("CREATE",C5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C5" xr:uid="{304DA74F-3195-45E6-B4AE-3659A1838A51}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{304DA74F-3195-45E6-B4AE-3659A1838A51}">
       <formula1>"CREATE,NOACTION"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1204,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124A7D2A-96B3-445A-854B-E4145A8C05CC}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2218,7 +2133,7 @@
         <v>165</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2227,130 +2142,6 @@
       </c>
       <c r="B127" s="2">
         <v>9000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E574417C-4FA0-4012-9599-E24A146FF4B8}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="2">
-        <v>31000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="2">
-        <v>31000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="2">
-        <v>31000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="2">
-        <v>31000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>